<commit_message>
new@3.0.1#:add total sheets and modify decovery's sheet
</commit_message>
<xml_diff>
--- a/VersionRecords/Version3.0.1/版本Bug和特性计划及评审表v3.0.1_发现组.xlsx
+++ b/VersionRecords/Version3.0.1/版本Bug和特性计划及评审表v3.0.1_发现组.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\mogo_git\Mogo_Doc\VersionRecords\Version3.0.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Test\Mogo_Doc\VersionRecords\Version3.0.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="45">
   <si>
     <t>No</t>
   </si>
@@ -171,6 +171,18 @@
   </si>
   <si>
     <t>吕崇新</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>发现组</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否影响数据</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>否</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -842,36 +854,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S218"/>
+  <dimension ref="A1:T218"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5" style="19" customWidth="1"/>
-    <col min="2" max="2" width="44.25" style="20" customWidth="1"/>
-    <col min="3" max="3" width="22.5" style="19" customWidth="1"/>
-    <col min="4" max="4" width="22.75" style="19" customWidth="1"/>
-    <col min="5" max="5" width="9.75" style="19" customWidth="1"/>
-    <col min="6" max="6" width="12.25" style="20" customWidth="1"/>
-    <col min="7" max="7" width="9.75" style="19" customWidth="1"/>
-    <col min="8" max="8" width="11.625" style="20" customWidth="1"/>
-    <col min="9" max="9" width="12.875" style="20" customWidth="1"/>
-    <col min="10" max="10" width="23.875" style="19" customWidth="1"/>
-    <col min="11" max="12" width="11.875" style="19" customWidth="1"/>
+    <col min="1" max="1" width="3.44140625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="44.21875" style="20" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" style="19" customWidth="1"/>
+    <col min="4" max="4" width="22.77734375" style="19" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" style="19" customWidth="1"/>
+    <col min="6" max="6" width="12.21875" style="20" customWidth="1"/>
+    <col min="7" max="7" width="9.77734375" style="19" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" style="20" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" style="20" customWidth="1"/>
+    <col min="10" max="10" width="23.88671875" style="19" customWidth="1"/>
+    <col min="11" max="12" width="11.88671875" style="19" customWidth="1"/>
     <col min="13" max="13" width="9" style="20"/>
-    <col min="14" max="14" width="11.625" style="20" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.625" style="20" customWidth="1"/>
-    <col min="16" max="16" width="12.125" style="23" customWidth="1"/>
-    <col min="17" max="17" width="17.625" style="23" customWidth="1"/>
-    <col min="18" max="18" width="48.5" style="20" customWidth="1"/>
-    <col min="19" max="19" width="8.875" customWidth="1"/>
-    <col min="20" max="16384" width="9" style="2"/>
+    <col min="14" max="14" width="11.6640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" style="20" customWidth="1"/>
+    <col min="16" max="16" width="12.109375" style="23" customWidth="1"/>
+    <col min="17" max="18" width="17.6640625" style="23" customWidth="1"/>
+    <col min="19" max="19" width="48.44140625" style="20" customWidth="1"/>
+    <col min="20" max="20" width="8.88671875" customWidth="1"/>
+    <col min="21" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="1" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -924,10 +936,13 @@
         <v>18</v>
       </c>
       <c r="R1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="A2" s="21">
         <v>1</v>
       </c>
@@ -956,7 +971,9 @@
       <c r="J2" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="12"/>
+      <c r="K2" s="12" t="s">
+        <v>42</v>
+      </c>
       <c r="L2" s="12"/>
       <c r="M2" s="14"/>
       <c r="N2" s="13"/>
@@ -965,10 +982,13 @@
         <v>1202</v>
       </c>
       <c r="Q2" s="22"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="10"/>
-    </row>
-    <row r="3" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R2" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="S2" s="18"/>
+      <c r="T2" s="10"/>
+    </row>
+    <row r="3" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="A3" s="21">
         <v>2</v>
       </c>
@@ -997,7 +1017,9 @@
       <c r="J3" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="12"/>
+      <c r="K3" s="12" t="s">
+        <v>42</v>
+      </c>
       <c r="L3" s="12"/>
       <c r="M3" s="14"/>
       <c r="N3" s="13"/>
@@ -1006,10 +1028,13 @@
         <v>1217</v>
       </c>
       <c r="Q3" s="22"/>
-      <c r="R3" s="18"/>
-      <c r="S3" s="10"/>
-    </row>
-    <row r="4" spans="1:19" s="11" customFormat="1" ht="33" x14ac:dyDescent="0.35">
+      <c r="R3" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="S3" s="18"/>
+      <c r="T3" s="10"/>
+    </row>
+    <row r="4" spans="1:20" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A4" s="21">
         <v>3</v>
       </c>
@@ -1038,7 +1063,9 @@
       <c r="J4" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="K4" s="12"/>
+      <c r="K4" s="12" t="s">
+        <v>42</v>
+      </c>
       <c r="L4" s="12"/>
       <c r="M4" s="14"/>
       <c r="N4" s="13"/>
@@ -1047,10 +1074,13 @@
         <v>827</v>
       </c>
       <c r="Q4" s="22"/>
-      <c r="R4" s="18"/>
-      <c r="S4" s="10"/>
-    </row>
-    <row r="5" spans="1:19" s="11" customFormat="1" ht="33" x14ac:dyDescent="0.35">
+      <c r="R4" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="S4" s="18"/>
+      <c r="T4" s="10"/>
+    </row>
+    <row r="5" spans="1:20" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A5" s="21">
         <v>4</v>
       </c>
@@ -1079,7 +1109,9 @@
       <c r="J5" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="K5" s="12"/>
+      <c r="K5" s="12" t="s">
+        <v>42</v>
+      </c>
       <c r="L5" s="12"/>
       <c r="M5" s="14"/>
       <c r="N5" s="13"/>
@@ -1088,10 +1120,13 @@
         <v>919</v>
       </c>
       <c r="Q5" s="22"/>
-      <c r="R5" s="18"/>
-      <c r="S5" s="10"/>
-    </row>
-    <row r="6" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R5" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="S5" s="18"/>
+      <c r="T5" s="10"/>
+    </row>
+    <row r="6" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="A6" s="21">
         <v>5</v>
       </c>
@@ -1120,7 +1155,9 @@
       <c r="J6" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="K6" s="12"/>
+      <c r="K6" s="12" t="s">
+        <v>42</v>
+      </c>
       <c r="L6" s="12"/>
       <c r="M6" s="14"/>
       <c r="N6" s="13"/>
@@ -1129,10 +1166,13 @@
         <v>1220</v>
       </c>
       <c r="Q6" s="22"/>
-      <c r="R6" s="18"/>
-      <c r="S6" s="10"/>
-    </row>
-    <row r="7" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R6" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="S6" s="18"/>
+      <c r="T6" s="10"/>
+    </row>
+    <row r="7" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="A7" s="21">
         <v>6</v>
       </c>
@@ -1161,7 +1201,9 @@
       <c r="J7" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="K7" s="12"/>
+      <c r="K7" s="12" t="s">
+        <v>42</v>
+      </c>
       <c r="L7" s="12"/>
       <c r="M7" s="14"/>
       <c r="N7" s="13"/>
@@ -1170,10 +1212,13 @@
         <v>1222</v>
       </c>
       <c r="Q7" s="22"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="10"/>
-    </row>
-    <row r="8" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R7" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="S7" s="18"/>
+      <c r="T7" s="10"/>
+    </row>
+    <row r="8" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="A8" s="21"/>
       <c r="B8" s="30"/>
       <c r="C8" s="12"/>
@@ -1191,10 +1236,11 @@
       <c r="O8" s="14"/>
       <c r="P8" s="22"/>
       <c r="Q8" s="22"/>
-      <c r="R8" s="18"/>
-      <c r="S8" s="10"/>
-    </row>
-    <row r="9" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R8" s="22"/>
+      <c r="S8" s="18"/>
+      <c r="T8" s="10"/>
+    </row>
+    <row r="9" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="A9" s="21"/>
       <c r="B9" s="30"/>
       <c r="C9" s="12"/>
@@ -1212,10 +1258,11 @@
       <c r="O9" s="14"/>
       <c r="P9" s="22"/>
       <c r="Q9" s="22"/>
-      <c r="R9" s="18"/>
-      <c r="S9" s="10"/>
-    </row>
-    <row r="10" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R9" s="22"/>
+      <c r="S9" s="18"/>
+      <c r="T9" s="10"/>
+    </row>
+    <row r="10" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="A10" s="21"/>
       <c r="B10" s="30"/>
       <c r="C10" s="12"/>
@@ -1233,10 +1280,11 @@
       <c r="O10" s="14"/>
       <c r="P10" s="22"/>
       <c r="Q10" s="22"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="10"/>
-    </row>
-    <row r="11" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R10" s="22"/>
+      <c r="S10" s="18"/>
+      <c r="T10" s="10"/>
+    </row>
+    <row r="11" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="A11" s="21"/>
       <c r="B11" s="30"/>
       <c r="C11" s="12"/>
@@ -1254,10 +1302,11 @@
       <c r="O11" s="14"/>
       <c r="P11" s="22"/>
       <c r="Q11" s="22"/>
-      <c r="R11" s="18"/>
-      <c r="S11" s="10"/>
-    </row>
-    <row r="12" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R11" s="22"/>
+      <c r="S11" s="18"/>
+      <c r="T11" s="10"/>
+    </row>
+    <row r="12" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="A12" s="21"/>
       <c r="B12" s="30"/>
       <c r="C12" s="12"/>
@@ -1275,10 +1324,11 @@
       <c r="O12" s="14"/>
       <c r="P12" s="22"/>
       <c r="Q12" s="22"/>
-      <c r="R12" s="18"/>
-      <c r="S12" s="10"/>
-    </row>
-    <row r="13" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R12" s="22"/>
+      <c r="S12" s="18"/>
+      <c r="T12" s="10"/>
+    </row>
+    <row r="13" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="A13" s="21"/>
       <c r="B13" s="30"/>
       <c r="C13" s="12"/>
@@ -1296,10 +1346,11 @@
       <c r="O13" s="14"/>
       <c r="P13" s="22"/>
       <c r="Q13" s="22"/>
-      <c r="R13" s="18"/>
-      <c r="S13" s="10"/>
-    </row>
-    <row r="14" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R13" s="22"/>
+      <c r="S13" s="18"/>
+      <c r="T13" s="10"/>
+    </row>
+    <row r="14" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="A14" s="21"/>
       <c r="B14" s="30"/>
       <c r="C14" s="12"/>
@@ -1317,10 +1368,11 @@
       <c r="O14" s="14"/>
       <c r="P14" s="22"/>
       <c r="Q14" s="22"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="10"/>
-    </row>
-    <row r="15" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R14" s="22"/>
+      <c r="S14" s="18"/>
+      <c r="T14" s="10"/>
+    </row>
+    <row r="15" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="A15" s="21"/>
       <c r="B15" s="30"/>
       <c r="C15" s="12"/>
@@ -1338,10 +1390,11 @@
       <c r="O15" s="14"/>
       <c r="P15" s="22"/>
       <c r="Q15" s="22"/>
-      <c r="R15" s="18"/>
-      <c r="S15" s="10"/>
-    </row>
-    <row r="16" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R15" s="22"/>
+      <c r="S15" s="18"/>
+      <c r="T15" s="10"/>
+    </row>
+    <row r="16" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="A16" s="21"/>
       <c r="B16" s="30"/>
       <c r="C16" s="12"/>
@@ -1359,10 +1412,11 @@
       <c r="O16" s="14"/>
       <c r="P16" s="22"/>
       <c r="Q16" s="22"/>
-      <c r="R16" s="18"/>
-      <c r="S16" s="10"/>
-    </row>
-    <row r="17" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R16" s="22"/>
+      <c r="S16" s="18"/>
+      <c r="T16" s="10"/>
+    </row>
+    <row r="17" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="A17" s="21"/>
       <c r="B17" s="30"/>
       <c r="C17" s="12"/>
@@ -1380,10 +1434,11 @@
       <c r="O17" s="14"/>
       <c r="P17" s="7"/>
       <c r="Q17" s="7"/>
-      <c r="R17" s="18"/>
-      <c r="S17" s="10"/>
-    </row>
-    <row r="18" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R17" s="7"/>
+      <c r="S17" s="18"/>
+      <c r="T17" s="10"/>
+    </row>
+    <row r="18" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="A18" s="21"/>
       <c r="B18" s="31"/>
       <c r="C18" s="12"/>
@@ -1401,10 +1456,11 @@
       <c r="O18" s="14"/>
       <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
-      <c r="R18" s="18"/>
-      <c r="S18" s="10"/>
-    </row>
-    <row r="19" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R18" s="7"/>
+      <c r="S18" s="18"/>
+      <c r="T18" s="10"/>
+    </row>
+    <row r="19" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="A19" s="21"/>
       <c r="B19" s="31"/>
       <c r="C19" s="12"/>
@@ -1422,10 +1478,11 @@
       <c r="O19" s="14"/>
       <c r="P19" s="7"/>
       <c r="Q19" s="7"/>
-      <c r="R19" s="18"/>
-      <c r="S19" s="10"/>
-    </row>
-    <row r="20" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R19" s="7"/>
+      <c r="S19" s="18"/>
+      <c r="T19" s="10"/>
+    </row>
+    <row r="20" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="21"/>
       <c r="B20" s="8"/>
       <c r="C20" s="12"/>
@@ -1443,10 +1500,11 @@
       <c r="O20" s="14"/>
       <c r="P20" s="7"/>
       <c r="Q20" s="7"/>
-      <c r="R20" s="18"/>
-      <c r="S20" s="10"/>
-    </row>
-    <row r="21" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R20" s="7"/>
+      <c r="S20" s="18"/>
+      <c r="T20" s="10"/>
+    </row>
+    <row r="21" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="21"/>
       <c r="B21" s="8"/>
       <c r="C21" s="12"/>
@@ -1464,10 +1522,11 @@
       <c r="O21" s="14"/>
       <c r="P21" s="7"/>
       <c r="Q21" s="7"/>
-      <c r="R21" s="18"/>
-      <c r="S21" s="10"/>
-    </row>
-    <row r="22" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R21" s="7"/>
+      <c r="S21" s="18"/>
+      <c r="T21" s="10"/>
+    </row>
+    <row r="22" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="21"/>
       <c r="B22" s="8"/>
       <c r="C22" s="12"/>
@@ -1485,10 +1544,11 @@
       <c r="O22" s="14"/>
       <c r="P22" s="7"/>
       <c r="Q22" s="7"/>
-      <c r="R22" s="18"/>
-      <c r="S22" s="10"/>
-    </row>
-    <row r="23" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R22" s="7"/>
+      <c r="S22" s="18"/>
+      <c r="T22" s="10"/>
+    </row>
+    <row r="23" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="21"/>
       <c r="B23" s="8"/>
       <c r="C23" s="12"/>
@@ -1506,10 +1566,11 @@
       <c r="O23" s="14"/>
       <c r="P23" s="7"/>
       <c r="Q23" s="7"/>
-      <c r="R23" s="18"/>
-      <c r="S23" s="10"/>
-    </row>
-    <row r="24" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R23" s="7"/>
+      <c r="S23" s="18"/>
+      <c r="T23" s="10"/>
+    </row>
+    <row r="24" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="21"/>
       <c r="B24" s="8"/>
       <c r="C24" s="12"/>
@@ -1527,10 +1588,11 @@
       <c r="O24" s="14"/>
       <c r="P24" s="7"/>
       <c r="Q24" s="7"/>
-      <c r="R24" s="18"/>
-      <c r="S24" s="10"/>
-    </row>
-    <row r="25" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R24" s="7"/>
+      <c r="S24" s="18"/>
+      <c r="T24" s="10"/>
+    </row>
+    <row r="25" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="21"/>
       <c r="B25" s="8"/>
       <c r="C25" s="12"/>
@@ -1548,10 +1610,11 @@
       <c r="O25" s="14"/>
       <c r="P25" s="7"/>
       <c r="Q25" s="7"/>
-      <c r="R25" s="18"/>
-      <c r="S25" s="10"/>
-    </row>
-    <row r="26" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R25" s="7"/>
+      <c r="S25" s="18"/>
+      <c r="T25" s="10"/>
+    </row>
+    <row r="26" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="21"/>
       <c r="B26" s="8"/>
       <c r="C26" s="12"/>
@@ -1569,10 +1632,11 @@
       <c r="O26" s="14"/>
       <c r="P26" s="7"/>
       <c r="Q26" s="7"/>
-      <c r="R26" s="18"/>
-      <c r="S26" s="10"/>
-    </row>
-    <row r="27" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R26" s="7"/>
+      <c r="S26" s="18"/>
+      <c r="T26" s="10"/>
+    </row>
+    <row r="27" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="21"/>
       <c r="B27" s="8"/>
       <c r="C27" s="12"/>
@@ -1590,10 +1654,11 @@
       <c r="O27" s="14"/>
       <c r="P27" s="7"/>
       <c r="Q27" s="7"/>
-      <c r="R27" s="18"/>
-      <c r="S27" s="10"/>
-    </row>
-    <row r="28" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R27" s="7"/>
+      <c r="S27" s="18"/>
+      <c r="T27" s="10"/>
+    </row>
+    <row r="28" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="21"/>
       <c r="B28" s="8"/>
       <c r="C28" s="12"/>
@@ -1611,10 +1676,11 @@
       <c r="O28" s="14"/>
       <c r="P28" s="7"/>
       <c r="Q28" s="7"/>
-      <c r="R28" s="18"/>
-      <c r="S28" s="10"/>
-    </row>
-    <row r="29" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R28" s="7"/>
+      <c r="S28" s="18"/>
+      <c r="T28" s="10"/>
+    </row>
+    <row r="29" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="21"/>
       <c r="B29" s="8"/>
       <c r="C29" s="12"/>
@@ -1632,10 +1698,11 @@
       <c r="O29" s="14"/>
       <c r="P29" s="7"/>
       <c r="Q29" s="7"/>
-      <c r="R29" s="18"/>
-      <c r="S29" s="10"/>
-    </row>
-    <row r="30" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R29" s="7"/>
+      <c r="S29" s="18"/>
+      <c r="T29" s="10"/>
+    </row>
+    <row r="30" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="21"/>
       <c r="B30" s="8"/>
       <c r="C30" s="12"/>
@@ -1653,10 +1720,11 @@
       <c r="O30" s="14"/>
       <c r="P30" s="7"/>
       <c r="Q30" s="7"/>
-      <c r="R30" s="18"/>
-      <c r="S30" s="10"/>
-    </row>
-    <row r="31" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R30" s="7"/>
+      <c r="S30" s="18"/>
+      <c r="T30" s="10"/>
+    </row>
+    <row r="31" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="21"/>
       <c r="B31" s="8"/>
       <c r="C31" s="12"/>
@@ -1674,10 +1742,11 @@
       <c r="O31" s="14"/>
       <c r="P31" s="7"/>
       <c r="Q31" s="7"/>
-      <c r="R31" s="18"/>
-      <c r="S31" s="10"/>
-    </row>
-    <row r="32" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R31" s="7"/>
+      <c r="S31" s="18"/>
+      <c r="T31" s="10"/>
+    </row>
+    <row r="32" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="21"/>
       <c r="B32" s="8"/>
       <c r="C32" s="12"/>
@@ -1695,10 +1764,11 @@
       <c r="O32" s="14"/>
       <c r="P32" s="7"/>
       <c r="Q32" s="7"/>
-      <c r="R32" s="18"/>
-      <c r="S32" s="10"/>
-    </row>
-    <row r="33" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R32" s="7"/>
+      <c r="S32" s="18"/>
+      <c r="T32" s="10"/>
+    </row>
+    <row r="33" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="21"/>
       <c r="B33" s="8"/>
       <c r="C33" s="12"/>
@@ -1716,10 +1786,11 @@
       <c r="O33" s="14"/>
       <c r="P33" s="7"/>
       <c r="Q33" s="7"/>
-      <c r="R33" s="18"/>
-      <c r="S33" s="10"/>
-    </row>
-    <row r="34" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R33" s="7"/>
+      <c r="S33" s="18"/>
+      <c r="T33" s="10"/>
+    </row>
+    <row r="34" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="21"/>
       <c r="B34" s="8"/>
       <c r="C34" s="12"/>
@@ -1737,10 +1808,11 @@
       <c r="O34" s="14"/>
       <c r="P34" s="7"/>
       <c r="Q34" s="7"/>
-      <c r="R34" s="18"/>
-      <c r="S34" s="10"/>
-    </row>
-    <row r="35" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R34" s="7"/>
+      <c r="S34" s="18"/>
+      <c r="T34" s="10"/>
+    </row>
+    <row r="35" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="21"/>
       <c r="B35" s="8"/>
       <c r="C35" s="12"/>
@@ -1758,10 +1830,11 @@
       <c r="O35" s="14"/>
       <c r="P35" s="7"/>
       <c r="Q35" s="7"/>
-      <c r="R35" s="18"/>
-      <c r="S35" s="10"/>
-    </row>
-    <row r="36" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R35" s="7"/>
+      <c r="S35" s="18"/>
+      <c r="T35" s="10"/>
+    </row>
+    <row r="36" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="21"/>
       <c r="B36" s="8"/>
       <c r="C36" s="12"/>
@@ -1779,10 +1852,11 @@
       <c r="O36" s="14"/>
       <c r="P36" s="7"/>
       <c r="Q36" s="7"/>
-      <c r="R36" s="18"/>
-      <c r="S36" s="10"/>
-    </row>
-    <row r="37" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R36" s="7"/>
+      <c r="S36" s="18"/>
+      <c r="T36" s="10"/>
+    </row>
+    <row r="37" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="21"/>
       <c r="B37" s="8"/>
       <c r="C37" s="12"/>
@@ -1800,10 +1874,11 @@
       <c r="O37" s="14"/>
       <c r="P37" s="7"/>
       <c r="Q37" s="7"/>
-      <c r="R37" s="18"/>
-      <c r="S37" s="10"/>
-    </row>
-    <row r="38" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R37" s="7"/>
+      <c r="S37" s="18"/>
+      <c r="T37" s="10"/>
+    </row>
+    <row r="38" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="21"/>
       <c r="B38" s="8"/>
       <c r="C38" s="12"/>
@@ -1821,10 +1896,11 @@
       <c r="O38" s="14"/>
       <c r="P38" s="7"/>
       <c r="Q38" s="7"/>
-      <c r="R38" s="18"/>
-      <c r="S38" s="10"/>
-    </row>
-    <row r="39" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R38" s="7"/>
+      <c r="S38" s="18"/>
+      <c r="T38" s="10"/>
+    </row>
+    <row r="39" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="21"/>
       <c r="B39" s="8"/>
       <c r="C39" s="12"/>
@@ -1842,10 +1918,11 @@
       <c r="O39" s="14"/>
       <c r="P39" s="7"/>
       <c r="Q39" s="7"/>
-      <c r="R39" s="18"/>
-      <c r="S39" s="10"/>
-    </row>
-    <row r="40" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R39" s="7"/>
+      <c r="S39" s="18"/>
+      <c r="T39" s="10"/>
+    </row>
+    <row r="40" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="21"/>
       <c r="B40" s="8"/>
       <c r="C40" s="12"/>
@@ -1863,10 +1940,11 @@
       <c r="O40" s="14"/>
       <c r="P40" s="7"/>
       <c r="Q40" s="7"/>
-      <c r="R40" s="18"/>
-      <c r="S40" s="10"/>
-    </row>
-    <row r="41" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R40" s="7"/>
+      <c r="S40" s="18"/>
+      <c r="T40" s="10"/>
+    </row>
+    <row r="41" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="21"/>
       <c r="B41" s="8"/>
       <c r="C41" s="12"/>
@@ -1884,10 +1962,11 @@
       <c r="O41" s="14"/>
       <c r="P41" s="7"/>
       <c r="Q41" s="7"/>
-      <c r="R41" s="18"/>
-      <c r="S41" s="10"/>
-    </row>
-    <row r="42" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R41" s="7"/>
+      <c r="S41" s="18"/>
+      <c r="T41" s="10"/>
+    </row>
+    <row r="42" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="21"/>
       <c r="B42" s="8"/>
       <c r="C42" s="12"/>
@@ -1905,10 +1984,11 @@
       <c r="O42" s="14"/>
       <c r="P42" s="7"/>
       <c r="Q42" s="7"/>
-      <c r="R42" s="18"/>
-      <c r="S42" s="10"/>
-    </row>
-    <row r="43" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R42" s="7"/>
+      <c r="S42" s="18"/>
+      <c r="T42" s="10"/>
+    </row>
+    <row r="43" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="21"/>
       <c r="B43" s="8"/>
       <c r="C43" s="12"/>
@@ -1926,10 +2006,11 @@
       <c r="O43" s="14"/>
       <c r="P43" s="7"/>
       <c r="Q43" s="7"/>
-      <c r="R43" s="18"/>
-      <c r="S43" s="10"/>
-    </row>
-    <row r="44" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R43" s="7"/>
+      <c r="S43" s="18"/>
+      <c r="T43" s="10"/>
+    </row>
+    <row r="44" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="21"/>
       <c r="B44" s="8"/>
       <c r="C44" s="12"/>
@@ -1947,10 +2028,11 @@
       <c r="O44" s="14"/>
       <c r="P44" s="7"/>
       <c r="Q44" s="7"/>
-      <c r="R44" s="18"/>
-      <c r="S44" s="10"/>
-    </row>
-    <row r="45" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R44" s="7"/>
+      <c r="S44" s="18"/>
+      <c r="T44" s="10"/>
+    </row>
+    <row r="45" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="21"/>
       <c r="B45" s="8"/>
       <c r="C45" s="12"/>
@@ -1968,10 +2050,11 @@
       <c r="O45" s="14"/>
       <c r="P45" s="7"/>
       <c r="Q45" s="7"/>
-      <c r="R45" s="18"/>
-      <c r="S45" s="10"/>
-    </row>
-    <row r="46" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R45" s="7"/>
+      <c r="S45" s="18"/>
+      <c r="T45" s="10"/>
+    </row>
+    <row r="46" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="21"/>
       <c r="B46" s="8"/>
       <c r="C46" s="12"/>
@@ -1989,10 +2072,11 @@
       <c r="O46" s="14"/>
       <c r="P46" s="7"/>
       <c r="Q46" s="7"/>
-      <c r="R46" s="18"/>
-      <c r="S46" s="10"/>
-    </row>
-    <row r="47" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R46" s="7"/>
+      <c r="S46" s="18"/>
+      <c r="T46" s="10"/>
+    </row>
+    <row r="47" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="21"/>
       <c r="B47" s="8"/>
       <c r="C47" s="12"/>
@@ -2010,10 +2094,11 @@
       <c r="O47" s="14"/>
       <c r="P47" s="7"/>
       <c r="Q47" s="7"/>
-      <c r="R47" s="18"/>
-      <c r="S47" s="10"/>
-    </row>
-    <row r="48" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R47" s="7"/>
+      <c r="S47" s="18"/>
+      <c r="T47" s="10"/>
+    </row>
+    <row r="48" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="21"/>
       <c r="B48" s="8"/>
       <c r="C48" s="12"/>
@@ -2031,10 +2116,11 @@
       <c r="O48" s="14"/>
       <c r="P48" s="7"/>
       <c r="Q48" s="7"/>
-      <c r="R48" s="18"/>
-      <c r="S48" s="10"/>
-    </row>
-    <row r="49" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R48" s="7"/>
+      <c r="S48" s="18"/>
+      <c r="T48" s="10"/>
+    </row>
+    <row r="49" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="21"/>
       <c r="B49" s="8"/>
       <c r="C49" s="12"/>
@@ -2052,10 +2138,11 @@
       <c r="O49" s="14"/>
       <c r="P49" s="7"/>
       <c r="Q49" s="7"/>
-      <c r="R49" s="18"/>
-      <c r="S49" s="10"/>
-    </row>
-    <row r="50" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R49" s="7"/>
+      <c r="S49" s="18"/>
+      <c r="T49" s="10"/>
+    </row>
+    <row r="50" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="21"/>
       <c r="B50" s="8"/>
       <c r="C50" s="12"/>
@@ -2073,10 +2160,11 @@
       <c r="O50" s="14"/>
       <c r="P50" s="7"/>
       <c r="Q50" s="7"/>
-      <c r="R50" s="18"/>
-      <c r="S50" s="10"/>
-    </row>
-    <row r="51" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R50" s="7"/>
+      <c r="S50" s="18"/>
+      <c r="T50" s="10"/>
+    </row>
+    <row r="51" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="21"/>
       <c r="B51" s="8"/>
       <c r="C51" s="12"/>
@@ -2094,10 +2182,11 @@
       <c r="O51" s="14"/>
       <c r="P51" s="7"/>
       <c r="Q51" s="7"/>
-      <c r="R51" s="18"/>
-      <c r="S51" s="10"/>
-    </row>
-    <row r="52" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R51" s="7"/>
+      <c r="S51" s="18"/>
+      <c r="T51" s="10"/>
+    </row>
+    <row r="52" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="21"/>
       <c r="B52" s="8"/>
       <c r="C52" s="12"/>
@@ -2115,10 +2204,11 @@
       <c r="O52" s="14"/>
       <c r="P52" s="7"/>
       <c r="Q52" s="7"/>
-      <c r="R52" s="18"/>
-      <c r="S52" s="10"/>
-    </row>
-    <row r="53" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R52" s="7"/>
+      <c r="S52" s="18"/>
+      <c r="T52" s="10"/>
+    </row>
+    <row r="53" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="21"/>
       <c r="B53" s="8"/>
       <c r="C53" s="12"/>
@@ -2136,10 +2226,11 @@
       <c r="O53" s="14"/>
       <c r="P53" s="7"/>
       <c r="Q53" s="7"/>
-      <c r="R53" s="18"/>
-      <c r="S53" s="10"/>
-    </row>
-    <row r="54" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R53" s="7"/>
+      <c r="S53" s="18"/>
+      <c r="T53" s="10"/>
+    </row>
+    <row r="54" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="21"/>
       <c r="B54" s="8"/>
       <c r="C54" s="12"/>
@@ -2157,10 +2248,11 @@
       <c r="O54" s="14"/>
       <c r="P54" s="7"/>
       <c r="Q54" s="7"/>
-      <c r="R54" s="18"/>
-      <c r="S54" s="10"/>
-    </row>
-    <row r="55" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R54" s="7"/>
+      <c r="S54" s="18"/>
+      <c r="T54" s="10"/>
+    </row>
+    <row r="55" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="21"/>
       <c r="B55" s="8"/>
       <c r="C55" s="12"/>
@@ -2178,10 +2270,11 @@
       <c r="O55" s="14"/>
       <c r="P55" s="7"/>
       <c r="Q55" s="7"/>
-      <c r="R55" s="18"/>
-      <c r="S55" s="10"/>
-    </row>
-    <row r="56" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R55" s="7"/>
+      <c r="S55" s="18"/>
+      <c r="T55" s="10"/>
+    </row>
+    <row r="56" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="21"/>
       <c r="B56" s="8"/>
       <c r="C56" s="12"/>
@@ -2199,10 +2292,11 @@
       <c r="O56" s="14"/>
       <c r="P56" s="7"/>
       <c r="Q56" s="7"/>
-      <c r="R56" s="18"/>
-      <c r="S56" s="10"/>
-    </row>
-    <row r="57" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R56" s="7"/>
+      <c r="S56" s="18"/>
+      <c r="T56" s="10"/>
+    </row>
+    <row r="57" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="21"/>
       <c r="B57" s="8"/>
       <c r="C57" s="12"/>
@@ -2220,10 +2314,11 @@
       <c r="O57" s="14"/>
       <c r="P57" s="7"/>
       <c r="Q57" s="7"/>
-      <c r="R57" s="18"/>
-      <c r="S57" s="10"/>
-    </row>
-    <row r="58" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R57" s="7"/>
+      <c r="S57" s="18"/>
+      <c r="T57" s="10"/>
+    </row>
+    <row r="58" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="21"/>
       <c r="B58" s="8"/>
       <c r="C58" s="12"/>
@@ -2241,10 +2336,11 @@
       <c r="O58" s="14"/>
       <c r="P58" s="7"/>
       <c r="Q58" s="7"/>
-      <c r="R58" s="18"/>
-      <c r="S58" s="10"/>
-    </row>
-    <row r="59" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R58" s="7"/>
+      <c r="S58" s="18"/>
+      <c r="T58" s="10"/>
+    </row>
+    <row r="59" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="21"/>
       <c r="B59" s="8"/>
       <c r="C59" s="12"/>
@@ -2262,10 +2358,11 @@
       <c r="O59" s="14"/>
       <c r="P59" s="7"/>
       <c r="Q59" s="7"/>
-      <c r="R59" s="18"/>
-      <c r="S59" s="10"/>
-    </row>
-    <row r="60" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R59" s="7"/>
+      <c r="S59" s="18"/>
+      <c r="T59" s="10"/>
+    </row>
+    <row r="60" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="21"/>
       <c r="B60" s="8"/>
       <c r="C60" s="12"/>
@@ -2283,10 +2380,11 @@
       <c r="O60" s="14"/>
       <c r="P60" s="7"/>
       <c r="Q60" s="7"/>
-      <c r="R60" s="18"/>
-      <c r="S60" s="10"/>
-    </row>
-    <row r="61" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R60" s="7"/>
+      <c r="S60" s="18"/>
+      <c r="T60" s="10"/>
+    </row>
+    <row r="61" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="9"/>
       <c r="B61" s="17"/>
       <c r="C61" s="9"/>
@@ -2304,10 +2402,11 @@
       <c r="O61" s="17"/>
       <c r="P61" s="7"/>
       <c r="Q61" s="7"/>
-      <c r="R61" s="17"/>
-      <c r="S61" s="10"/>
-    </row>
-    <row r="62" spans="1:19" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R61" s="7"/>
+      <c r="S61" s="17"/>
+      <c r="T61" s="10"/>
+    </row>
+    <row r="62" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="9"/>
       <c r="B62" s="17"/>
       <c r="C62" s="9"/>
@@ -2325,10 +2424,11 @@
       <c r="O62" s="17"/>
       <c r="P62" s="7"/>
       <c r="Q62" s="7"/>
-      <c r="R62" s="17"/>
-      <c r="S62" s="10"/>
-    </row>
-    <row r="63" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R62" s="7"/>
+      <c r="S62" s="17"/>
+      <c r="T62" s="10"/>
+    </row>
+    <row r="63" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="7"/>
       <c r="B63" s="4"/>
       <c r="C63" s="7"/>
@@ -2346,9 +2446,10 @@
       <c r="O63" s="4"/>
       <c r="P63" s="7"/>
       <c r="Q63" s="7"/>
-      <c r="R63" s="4"/>
-    </row>
-    <row r="64" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R63" s="7"/>
+      <c r="S63" s="4"/>
+    </row>
+    <row r="64" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="7"/>
       <c r="B64" s="4"/>
       <c r="C64" s="7"/>
@@ -2366,9 +2467,10 @@
       <c r="O64" s="4"/>
       <c r="P64" s="7"/>
       <c r="Q64" s="7"/>
-      <c r="R64" s="4"/>
-    </row>
-    <row r="65" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R64" s="7"/>
+      <c r="S64" s="4"/>
+    </row>
+    <row r="65" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="7"/>
       <c r="B65" s="4"/>
       <c r="C65" s="7"/>
@@ -2386,9 +2488,10 @@
       <c r="O65" s="4"/>
       <c r="P65" s="7"/>
       <c r="Q65" s="7"/>
-      <c r="R65" s="4"/>
-    </row>
-    <row r="66" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R65" s="7"/>
+      <c r="S65" s="4"/>
+    </row>
+    <row r="66" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="7"/>
       <c r="B66" s="4"/>
       <c r="C66" s="7"/>
@@ -2406,9 +2509,10 @@
       <c r="O66" s="4"/>
       <c r="P66" s="7"/>
       <c r="Q66" s="7"/>
-      <c r="R66" s="4"/>
-    </row>
-    <row r="67" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R66" s="7"/>
+      <c r="S66" s="4"/>
+    </row>
+    <row r="67" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="7"/>
       <c r="B67" s="4"/>
       <c r="C67" s="7"/>
@@ -2426,9 +2530,10 @@
       <c r="O67" s="4"/>
       <c r="P67" s="7"/>
       <c r="Q67" s="7"/>
-      <c r="R67" s="4"/>
-    </row>
-    <row r="68" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R67" s="7"/>
+      <c r="S67" s="4"/>
+    </row>
+    <row r="68" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="7"/>
       <c r="B68" s="4"/>
       <c r="C68" s="7"/>
@@ -2446,9 +2551,10 @@
       <c r="O68" s="4"/>
       <c r="P68" s="7"/>
       <c r="Q68" s="7"/>
-      <c r="R68" s="4"/>
-    </row>
-    <row r="69" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R68" s="7"/>
+      <c r="S68" s="4"/>
+    </row>
+    <row r="69" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="7"/>
       <c r="B69" s="4"/>
       <c r="C69" s="7"/>
@@ -2466,9 +2572,10 @@
       <c r="O69" s="4"/>
       <c r="P69" s="7"/>
       <c r="Q69" s="7"/>
-      <c r="R69" s="4"/>
-    </row>
-    <row r="70" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R69" s="7"/>
+      <c r="S69" s="4"/>
+    </row>
+    <row r="70" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="7"/>
       <c r="B70" s="4"/>
       <c r="C70" s="7"/>
@@ -2486,9 +2593,10 @@
       <c r="O70" s="4"/>
       <c r="P70" s="7"/>
       <c r="Q70" s="7"/>
-      <c r="R70" s="4"/>
-    </row>
-    <row r="71" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R70" s="7"/>
+      <c r="S70" s="4"/>
+    </row>
+    <row r="71" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="7"/>
       <c r="B71" s="4"/>
       <c r="C71" s="7"/>
@@ -2506,9 +2614,10 @@
       <c r="O71" s="4"/>
       <c r="P71" s="7"/>
       <c r="Q71" s="7"/>
-      <c r="R71" s="4"/>
-    </row>
-    <row r="72" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R71" s="7"/>
+      <c r="S71" s="4"/>
+    </row>
+    <row r="72" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="7"/>
       <c r="B72" s="4"/>
       <c r="C72" s="7"/>
@@ -2526,9 +2635,10 @@
       <c r="O72" s="4"/>
       <c r="P72" s="7"/>
       <c r="Q72" s="7"/>
-      <c r="R72" s="4"/>
-    </row>
-    <row r="73" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R72" s="7"/>
+      <c r="S72" s="4"/>
+    </row>
+    <row r="73" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="7"/>
       <c r="B73" s="4"/>
       <c r="C73" s="7"/>
@@ -2546,9 +2656,10 @@
       <c r="O73" s="4"/>
       <c r="P73" s="7"/>
       <c r="Q73" s="7"/>
-      <c r="R73" s="4"/>
-    </row>
-    <row r="74" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R73" s="7"/>
+      <c r="S73" s="4"/>
+    </row>
+    <row r="74" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="7"/>
       <c r="B74" s="4"/>
       <c r="C74" s="7"/>
@@ -2566,9 +2677,10 @@
       <c r="O74" s="4"/>
       <c r="P74" s="7"/>
       <c r="Q74" s="7"/>
-      <c r="R74" s="4"/>
-    </row>
-    <row r="75" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R74" s="7"/>
+      <c r="S74" s="4"/>
+    </row>
+    <row r="75" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="7"/>
       <c r="B75" s="4"/>
       <c r="C75" s="7"/>
@@ -2586,9 +2698,10 @@
       <c r="O75" s="4"/>
       <c r="P75" s="7"/>
       <c r="Q75" s="7"/>
-      <c r="R75" s="4"/>
-    </row>
-    <row r="76" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R75" s="7"/>
+      <c r="S75" s="4"/>
+    </row>
+    <row r="76" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="7"/>
       <c r="B76" s="4"/>
       <c r="C76" s="7"/>
@@ -2606,9 +2719,10 @@
       <c r="O76" s="4"/>
       <c r="P76" s="7"/>
       <c r="Q76" s="7"/>
-      <c r="R76" s="4"/>
-    </row>
-    <row r="77" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R76" s="7"/>
+      <c r="S76" s="4"/>
+    </row>
+    <row r="77" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="7"/>
       <c r="B77" s="4"/>
       <c r="C77" s="7"/>
@@ -2626,9 +2740,10 @@
       <c r="O77" s="4"/>
       <c r="P77" s="7"/>
       <c r="Q77" s="7"/>
-      <c r="R77" s="4"/>
-    </row>
-    <row r="78" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R77" s="7"/>
+      <c r="S77" s="4"/>
+    </row>
+    <row r="78" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="7"/>
       <c r="B78" s="4"/>
       <c r="C78" s="7"/>
@@ -2646,9 +2761,10 @@
       <c r="O78" s="4"/>
       <c r="P78" s="7"/>
       <c r="Q78" s="7"/>
-      <c r="R78" s="4"/>
-    </row>
-    <row r="79" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R78" s="7"/>
+      <c r="S78" s="4"/>
+    </row>
+    <row r="79" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="7"/>
       <c r="B79" s="4"/>
       <c r="C79" s="7"/>
@@ -2666,9 +2782,10 @@
       <c r="O79" s="4"/>
       <c r="P79" s="7"/>
       <c r="Q79" s="7"/>
-      <c r="R79" s="4"/>
-    </row>
-    <row r="80" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R79" s="7"/>
+      <c r="S79" s="4"/>
+    </row>
+    <row r="80" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="7"/>
       <c r="B80" s="4"/>
       <c r="C80" s="7"/>
@@ -2686,9 +2803,10 @@
       <c r="O80" s="4"/>
       <c r="P80" s="7"/>
       <c r="Q80" s="7"/>
-      <c r="R80" s="4"/>
-    </row>
-    <row r="81" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R80" s="7"/>
+      <c r="S80" s="4"/>
+    </row>
+    <row r="81" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="7"/>
       <c r="B81" s="4"/>
       <c r="C81" s="7"/>
@@ -2706,9 +2824,10 @@
       <c r="O81" s="4"/>
       <c r="P81" s="7"/>
       <c r="Q81" s="7"/>
-      <c r="R81" s="4"/>
-    </row>
-    <row r="82" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R81" s="7"/>
+      <c r="S81" s="4"/>
+    </row>
+    <row r="82" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="7"/>
       <c r="B82" s="4"/>
       <c r="C82" s="7"/>
@@ -2726,9 +2845,10 @@
       <c r="O82" s="4"/>
       <c r="P82" s="7"/>
       <c r="Q82" s="7"/>
-      <c r="R82" s="4"/>
-    </row>
-    <row r="83" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R82" s="7"/>
+      <c r="S82" s="4"/>
+    </row>
+    <row r="83" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="7"/>
       <c r="B83" s="4"/>
       <c r="C83" s="7"/>
@@ -2746,9 +2866,10 @@
       <c r="O83" s="4"/>
       <c r="P83" s="7"/>
       <c r="Q83" s="7"/>
-      <c r="R83" s="4"/>
-    </row>
-    <row r="84" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R83" s="7"/>
+      <c r="S83" s="4"/>
+    </row>
+    <row r="84" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="7"/>
       <c r="B84" s="4"/>
       <c r="C84" s="7"/>
@@ -2766,9 +2887,10 @@
       <c r="O84" s="4"/>
       <c r="P84" s="7"/>
       <c r="Q84" s="7"/>
-      <c r="R84" s="4"/>
-    </row>
-    <row r="85" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R84" s="7"/>
+      <c r="S84" s="4"/>
+    </row>
+    <row r="85" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="7"/>
       <c r="B85" s="4"/>
       <c r="C85" s="7"/>
@@ -2786,9 +2908,10 @@
       <c r="O85" s="4"/>
       <c r="P85" s="7"/>
       <c r="Q85" s="7"/>
-      <c r="R85" s="4"/>
-    </row>
-    <row r="86" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R85" s="7"/>
+      <c r="S85" s="4"/>
+    </row>
+    <row r="86" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="7"/>
       <c r="B86" s="4"/>
       <c r="C86" s="7"/>
@@ -2806,9 +2929,10 @@
       <c r="O86" s="4"/>
       <c r="P86" s="7"/>
       <c r="Q86" s="7"/>
-      <c r="R86" s="4"/>
-    </row>
-    <row r="87" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R86" s="7"/>
+      <c r="S86" s="4"/>
+    </row>
+    <row r="87" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="7"/>
       <c r="B87" s="4"/>
       <c r="C87" s="7"/>
@@ -2826,9 +2950,10 @@
       <c r="O87" s="4"/>
       <c r="P87" s="7"/>
       <c r="Q87" s="7"/>
-      <c r="R87" s="4"/>
-    </row>
-    <row r="88" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R87" s="7"/>
+      <c r="S87" s="4"/>
+    </row>
+    <row r="88" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="7"/>
       <c r="B88" s="4"/>
       <c r="C88" s="7"/>
@@ -2846,9 +2971,10 @@
       <c r="O88" s="4"/>
       <c r="P88" s="7"/>
       <c r="Q88" s="7"/>
-      <c r="R88" s="4"/>
-    </row>
-    <row r="89" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R88" s="7"/>
+      <c r="S88" s="4"/>
+    </row>
+    <row r="89" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="7"/>
       <c r="B89" s="4"/>
       <c r="C89" s="7"/>
@@ -2866,9 +2992,10 @@
       <c r="O89" s="4"/>
       <c r="P89" s="7"/>
       <c r="Q89" s="7"/>
-      <c r="R89" s="4"/>
-    </row>
-    <row r="90" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R89" s="7"/>
+      <c r="S89" s="4"/>
+    </row>
+    <row r="90" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="7"/>
       <c r="B90" s="4"/>
       <c r="C90" s="7"/>
@@ -2886,9 +3013,10 @@
       <c r="O90" s="4"/>
       <c r="P90" s="7"/>
       <c r="Q90" s="7"/>
-      <c r="R90" s="4"/>
-    </row>
-    <row r="91" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R90" s="7"/>
+      <c r="S90" s="4"/>
+    </row>
+    <row r="91" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="7"/>
       <c r="B91" s="4"/>
       <c r="C91" s="7"/>
@@ -2906,9 +3034,10 @@
       <c r="O91" s="4"/>
       <c r="P91" s="7"/>
       <c r="Q91" s="7"/>
-      <c r="R91" s="4"/>
-    </row>
-    <row r="92" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R91" s="7"/>
+      <c r="S91" s="4"/>
+    </row>
+    <row r="92" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="7"/>
       <c r="B92" s="4"/>
       <c r="C92" s="7"/>
@@ -2926,9 +3055,10 @@
       <c r="O92" s="4"/>
       <c r="P92" s="7"/>
       <c r="Q92" s="7"/>
-      <c r="R92" s="4"/>
-    </row>
-    <row r="93" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R92" s="7"/>
+      <c r="S92" s="4"/>
+    </row>
+    <row r="93" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="7"/>
       <c r="B93" s="4"/>
       <c r="C93" s="7"/>
@@ -2946,9 +3076,10 @@
       <c r="O93" s="4"/>
       <c r="P93" s="7"/>
       <c r="Q93" s="7"/>
-      <c r="R93" s="4"/>
-    </row>
-    <row r="94" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R93" s="7"/>
+      <c r="S93" s="4"/>
+    </row>
+    <row r="94" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="7"/>
       <c r="B94" s="4"/>
       <c r="C94" s="7"/>
@@ -2966,9 +3097,10 @@
       <c r="O94" s="4"/>
       <c r="P94" s="7"/>
       <c r="Q94" s="7"/>
-      <c r="R94" s="4"/>
-    </row>
-    <row r="95" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R94" s="7"/>
+      <c r="S94" s="4"/>
+    </row>
+    <row r="95" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="7"/>
       <c r="B95" s="4"/>
       <c r="C95" s="7"/>
@@ -2986,9 +3118,10 @@
       <c r="O95" s="4"/>
       <c r="P95" s="7"/>
       <c r="Q95" s="7"/>
-      <c r="R95" s="4"/>
-    </row>
-    <row r="96" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R95" s="7"/>
+      <c r="S95" s="4"/>
+    </row>
+    <row r="96" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="7"/>
       <c r="B96" s="4"/>
       <c r="C96" s="7"/>
@@ -3006,9 +3139,10 @@
       <c r="O96" s="4"/>
       <c r="P96" s="7"/>
       <c r="Q96" s="7"/>
-      <c r="R96" s="4"/>
-    </row>
-    <row r="97" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R96" s="7"/>
+      <c r="S96" s="4"/>
+    </row>
+    <row r="97" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="7"/>
       <c r="B97" s="4"/>
       <c r="C97" s="7"/>
@@ -3026,9 +3160,10 @@
       <c r="O97" s="4"/>
       <c r="P97" s="7"/>
       <c r="Q97" s="7"/>
-      <c r="R97" s="4"/>
-    </row>
-    <row r="98" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R97" s="7"/>
+      <c r="S97" s="4"/>
+    </row>
+    <row r="98" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="7"/>
       <c r="B98" s="4"/>
       <c r="C98" s="7"/>
@@ -3046,9 +3181,10 @@
       <c r="O98" s="4"/>
       <c r="P98" s="7"/>
       <c r="Q98" s="7"/>
-      <c r="R98" s="4"/>
-    </row>
-    <row r="99" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R98" s="7"/>
+      <c r="S98" s="4"/>
+    </row>
+    <row r="99" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="7"/>
       <c r="B99" s="4"/>
       <c r="C99" s="7"/>
@@ -3066,9 +3202,10 @@
       <c r="O99" s="4"/>
       <c r="P99" s="7"/>
       <c r="Q99" s="7"/>
-      <c r="R99" s="4"/>
-    </row>
-    <row r="100" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R99" s="7"/>
+      <c r="S99" s="4"/>
+    </row>
+    <row r="100" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="7"/>
       <c r="B100" s="4"/>
       <c r="C100" s="7"/>
@@ -3086,9 +3223,10 @@
       <c r="O100" s="4"/>
       <c r="P100" s="7"/>
       <c r="Q100" s="7"/>
-      <c r="R100" s="4"/>
-    </row>
-    <row r="101" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R100" s="7"/>
+      <c r="S100" s="4"/>
+    </row>
+    <row r="101" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="7"/>
       <c r="B101" s="4"/>
       <c r="C101" s="7"/>
@@ -3106,9 +3244,10 @@
       <c r="O101" s="4"/>
       <c r="P101" s="7"/>
       <c r="Q101" s="7"/>
-      <c r="R101" s="4"/>
-    </row>
-    <row r="102" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R101" s="7"/>
+      <c r="S101" s="4"/>
+    </row>
+    <row r="102" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="7"/>
       <c r="B102" s="4"/>
       <c r="C102" s="7"/>
@@ -3126,9 +3265,10 @@
       <c r="O102" s="4"/>
       <c r="P102" s="7"/>
       <c r="Q102" s="7"/>
-      <c r="R102" s="4"/>
-    </row>
-    <row r="103" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R102" s="7"/>
+      <c r="S102" s="4"/>
+    </row>
+    <row r="103" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="7"/>
       <c r="B103" s="4"/>
       <c r="C103" s="7"/>
@@ -3146,9 +3286,10 @@
       <c r="O103" s="4"/>
       <c r="P103" s="7"/>
       <c r="Q103" s="7"/>
-      <c r="R103" s="4"/>
-    </row>
-    <row r="104" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R103" s="7"/>
+      <c r="S103" s="4"/>
+    </row>
+    <row r="104" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="7"/>
       <c r="B104" s="4"/>
       <c r="C104" s="7"/>
@@ -3166,9 +3307,10 @@
       <c r="O104" s="4"/>
       <c r="P104" s="7"/>
       <c r="Q104" s="7"/>
-      <c r="R104" s="4"/>
-    </row>
-    <row r="105" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R104" s="7"/>
+      <c r="S104" s="4"/>
+    </row>
+    <row r="105" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" s="7"/>
       <c r="B105" s="4"/>
       <c r="C105" s="7"/>
@@ -3186,9 +3328,10 @@
       <c r="O105" s="4"/>
       <c r="P105" s="7"/>
       <c r="Q105" s="7"/>
-      <c r="R105" s="4"/>
-    </row>
-    <row r="106" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R105" s="7"/>
+      <c r="S105" s="4"/>
+    </row>
+    <row r="106" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="7"/>
       <c r="B106" s="4"/>
       <c r="C106" s="7"/>
@@ -3206,9 +3349,10 @@
       <c r="O106" s="4"/>
       <c r="P106" s="7"/>
       <c r="Q106" s="7"/>
-      <c r="R106" s="4"/>
-    </row>
-    <row r="107" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R106" s="7"/>
+      <c r="S106" s="4"/>
+    </row>
+    <row r="107" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" s="7"/>
       <c r="B107" s="4"/>
       <c r="C107" s="7"/>
@@ -3226,9 +3370,10 @@
       <c r="O107" s="4"/>
       <c r="P107" s="7"/>
       <c r="Q107" s="7"/>
-      <c r="R107" s="4"/>
-    </row>
-    <row r="108" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R107" s="7"/>
+      <c r="S107" s="4"/>
+    </row>
+    <row r="108" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A108" s="7"/>
       <c r="B108" s="4"/>
       <c r="C108" s="7"/>
@@ -3246,9 +3391,10 @@
       <c r="O108" s="4"/>
       <c r="P108" s="7"/>
       <c r="Q108" s="7"/>
-      <c r="R108" s="4"/>
-    </row>
-    <row r="109" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R108" s="7"/>
+      <c r="S108" s="4"/>
+    </row>
+    <row r="109" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A109" s="7"/>
       <c r="B109" s="4"/>
       <c r="C109" s="7"/>
@@ -3266,9 +3412,10 @@
       <c r="O109" s="4"/>
       <c r="P109" s="7"/>
       <c r="Q109" s="7"/>
-      <c r="R109" s="4"/>
-    </row>
-    <row r="110" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R109" s="7"/>
+      <c r="S109" s="4"/>
+    </row>
+    <row r="110" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A110" s="7"/>
       <c r="B110" s="4"/>
       <c r="C110" s="7"/>
@@ -3286,9 +3433,10 @@
       <c r="O110" s="4"/>
       <c r="P110" s="7"/>
       <c r="Q110" s="7"/>
-      <c r="R110" s="4"/>
-    </row>
-    <row r="111" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R110" s="7"/>
+      <c r="S110" s="4"/>
+    </row>
+    <row r="111" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A111" s="7"/>
       <c r="B111" s="4"/>
       <c r="C111" s="7"/>
@@ -3306,9 +3454,10 @@
       <c r="O111" s="4"/>
       <c r="P111" s="7"/>
       <c r="Q111" s="7"/>
-      <c r="R111" s="4"/>
-    </row>
-    <row r="112" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R111" s="7"/>
+      <c r="S111" s="4"/>
+    </row>
+    <row r="112" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A112" s="7"/>
       <c r="B112" s="4"/>
       <c r="C112" s="7"/>
@@ -3326,9 +3475,10 @@
       <c r="O112" s="4"/>
       <c r="P112" s="7"/>
       <c r="Q112" s="7"/>
-      <c r="R112" s="4"/>
-    </row>
-    <row r="113" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R112" s="7"/>
+      <c r="S112" s="4"/>
+    </row>
+    <row r="113" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A113" s="7"/>
       <c r="B113" s="4"/>
       <c r="C113" s="7"/>
@@ -3346,9 +3496,10 @@
       <c r="O113" s="4"/>
       <c r="P113" s="7"/>
       <c r="Q113" s="7"/>
-      <c r="R113" s="4"/>
-    </row>
-    <row r="114" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R113" s="7"/>
+      <c r="S113" s="4"/>
+    </row>
+    <row r="114" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A114" s="7"/>
       <c r="B114" s="4"/>
       <c r="C114" s="7"/>
@@ -3366,9 +3517,10 @@
       <c r="O114" s="4"/>
       <c r="P114" s="7"/>
       <c r="Q114" s="7"/>
-      <c r="R114" s="4"/>
-    </row>
-    <row r="115" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R114" s="7"/>
+      <c r="S114" s="4"/>
+    </row>
+    <row r="115" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A115" s="7"/>
       <c r="B115" s="4"/>
       <c r="C115" s="7"/>
@@ -3386,9 +3538,10 @@
       <c r="O115" s="4"/>
       <c r="P115" s="7"/>
       <c r="Q115" s="7"/>
-      <c r="R115" s="4"/>
-    </row>
-    <row r="116" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R115" s="7"/>
+      <c r="S115" s="4"/>
+    </row>
+    <row r="116" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A116" s="7"/>
       <c r="B116" s="4"/>
       <c r="C116" s="7"/>
@@ -3406,9 +3559,10 @@
       <c r="O116" s="4"/>
       <c r="P116" s="7"/>
       <c r="Q116" s="7"/>
-      <c r="R116" s="4"/>
-    </row>
-    <row r="117" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R116" s="7"/>
+      <c r="S116" s="4"/>
+    </row>
+    <row r="117" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A117" s="7"/>
       <c r="B117" s="4"/>
       <c r="C117" s="7"/>
@@ -3426,9 +3580,10 @@
       <c r="O117" s="4"/>
       <c r="P117" s="7"/>
       <c r="Q117" s="7"/>
-      <c r="R117" s="4"/>
-    </row>
-    <row r="118" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R117" s="7"/>
+      <c r="S117" s="4"/>
+    </row>
+    <row r="118" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A118" s="7"/>
       <c r="B118" s="4"/>
       <c r="C118" s="7"/>
@@ -3446,9 +3601,10 @@
       <c r="O118" s="4"/>
       <c r="P118" s="7"/>
       <c r="Q118" s="7"/>
-      <c r="R118" s="4"/>
-    </row>
-    <row r="119" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R118" s="7"/>
+      <c r="S118" s="4"/>
+    </row>
+    <row r="119" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A119" s="7"/>
       <c r="B119" s="4"/>
       <c r="C119" s="7"/>
@@ -3466,9 +3622,10 @@
       <c r="O119" s="4"/>
       <c r="P119" s="7"/>
       <c r="Q119" s="7"/>
-      <c r="R119" s="4"/>
-    </row>
-    <row r="120" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R119" s="7"/>
+      <c r="S119" s="4"/>
+    </row>
+    <row r="120" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A120" s="7"/>
       <c r="B120" s="4"/>
       <c r="C120" s="7"/>
@@ -3486,9 +3643,10 @@
       <c r="O120" s="4"/>
       <c r="P120" s="7"/>
       <c r="Q120" s="7"/>
-      <c r="R120" s="4"/>
-    </row>
-    <row r="121" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R120" s="7"/>
+      <c r="S120" s="4"/>
+    </row>
+    <row r="121" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A121" s="7"/>
       <c r="B121" s="4"/>
       <c r="C121" s="7"/>
@@ -3506,9 +3664,10 @@
       <c r="O121" s="4"/>
       <c r="P121" s="7"/>
       <c r="Q121" s="7"/>
-      <c r="R121" s="4"/>
-    </row>
-    <row r="122" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R121" s="7"/>
+      <c r="S121" s="4"/>
+    </row>
+    <row r="122" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A122" s="7"/>
       <c r="B122" s="4"/>
       <c r="C122" s="7"/>
@@ -3526,9 +3685,10 @@
       <c r="O122" s="4"/>
       <c r="P122" s="7"/>
       <c r="Q122" s="7"/>
-      <c r="R122" s="4"/>
-    </row>
-    <row r="123" spans="1:18" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="R122" s="7"/>
+      <c r="S122" s="4"/>
+    </row>
+    <row r="123" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A123" s="7"/>
       <c r="B123" s="4"/>
       <c r="C123" s="7"/>
@@ -3546,9 +3706,10 @@
       <c r="O123" s="4"/>
       <c r="P123" s="7"/>
       <c r="Q123" s="7"/>
-      <c r="R123" s="4"/>
-    </row>
-    <row r="124" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R123" s="7"/>
+      <c r="S123" s="4"/>
+    </row>
+    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A124" s="7"/>
       <c r="B124" s="4"/>
       <c r="C124" s="7"/>
@@ -3566,9 +3727,10 @@
       <c r="O124" s="4"/>
       <c r="P124" s="7"/>
       <c r="Q124" s="7"/>
-      <c r="R124" s="4"/>
-    </row>
-    <row r="125" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R124" s="7"/>
+      <c r="S124" s="4"/>
+    </row>
+    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A125" s="7"/>
       <c r="B125" s="4"/>
       <c r="C125" s="7"/>
@@ -3586,9 +3748,10 @@
       <c r="O125" s="4"/>
       <c r="P125" s="7"/>
       <c r="Q125" s="7"/>
-      <c r="R125" s="4"/>
-    </row>
-    <row r="126" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R125" s="7"/>
+      <c r="S125" s="4"/>
+    </row>
+    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A126" s="7"/>
       <c r="B126" s="4"/>
       <c r="C126" s="7"/>
@@ -3606,9 +3769,10 @@
       <c r="O126" s="4"/>
       <c r="P126" s="7"/>
       <c r="Q126" s="7"/>
-      <c r="R126" s="4"/>
-    </row>
-    <row r="127" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R126" s="7"/>
+      <c r="S126" s="4"/>
+    </row>
+    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A127" s="7"/>
       <c r="B127" s="4"/>
       <c r="C127" s="7"/>
@@ -3626,9 +3790,10 @@
       <c r="O127" s="4"/>
       <c r="P127" s="7"/>
       <c r="Q127" s="7"/>
-      <c r="R127" s="4"/>
-    </row>
-    <row r="128" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R127" s="7"/>
+      <c r="S127" s="4"/>
+    </row>
+    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A128" s="7"/>
       <c r="B128" s="4"/>
       <c r="C128" s="7"/>
@@ -3646,9 +3811,10 @@
       <c r="O128" s="4"/>
       <c r="P128" s="7"/>
       <c r="Q128" s="7"/>
-      <c r="R128" s="4"/>
-    </row>
-    <row r="129" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R128" s="7"/>
+      <c r="S128" s="4"/>
+    </row>
+    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A129" s="7"/>
       <c r="B129" s="4"/>
       <c r="C129" s="7"/>
@@ -3666,9 +3832,10 @@
       <c r="O129" s="4"/>
       <c r="P129" s="7"/>
       <c r="Q129" s="7"/>
-      <c r="R129" s="4"/>
-    </row>
-    <row r="130" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R129" s="7"/>
+      <c r="S129" s="4"/>
+    </row>
+    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A130" s="7"/>
       <c r="B130" s="4"/>
       <c r="C130" s="7"/>
@@ -3686,9 +3853,10 @@
       <c r="O130" s="4"/>
       <c r="P130" s="7"/>
       <c r="Q130" s="7"/>
-      <c r="R130" s="4"/>
-    </row>
-    <row r="131" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R130" s="7"/>
+      <c r="S130" s="4"/>
+    </row>
+    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A131" s="7"/>
       <c r="B131" s="4"/>
       <c r="C131" s="7"/>
@@ -3706,9 +3874,10 @@
       <c r="O131" s="4"/>
       <c r="P131" s="7"/>
       <c r="Q131" s="7"/>
-      <c r="R131" s="4"/>
-    </row>
-    <row r="132" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R131" s="7"/>
+      <c r="S131" s="4"/>
+    </row>
+    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A132" s="7"/>
       <c r="B132" s="4"/>
       <c r="C132" s="7"/>
@@ -3726,9 +3895,10 @@
       <c r="O132" s="4"/>
       <c r="P132" s="7"/>
       <c r="Q132" s="7"/>
-      <c r="R132" s="4"/>
-    </row>
-    <row r="133" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R132" s="7"/>
+      <c r="S132" s="4"/>
+    </row>
+    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A133" s="7"/>
       <c r="B133" s="4"/>
       <c r="C133" s="7"/>
@@ -3746,9 +3916,10 @@
       <c r="O133" s="4"/>
       <c r="P133" s="7"/>
       <c r="Q133" s="7"/>
-      <c r="R133" s="4"/>
-    </row>
-    <row r="134" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R133" s="7"/>
+      <c r="S133" s="4"/>
+    </row>
+    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A134" s="7"/>
       <c r="B134" s="4"/>
       <c r="C134" s="7"/>
@@ -3766,9 +3937,10 @@
       <c r="O134" s="4"/>
       <c r="P134" s="7"/>
       <c r="Q134" s="7"/>
-      <c r="R134" s="4"/>
-    </row>
-    <row r="135" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R134" s="7"/>
+      <c r="S134" s="4"/>
+    </row>
+    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A135" s="7"/>
       <c r="B135" s="4"/>
       <c r="C135" s="7"/>
@@ -3786,9 +3958,10 @@
       <c r="O135" s="4"/>
       <c r="P135" s="7"/>
       <c r="Q135" s="7"/>
-      <c r="R135" s="4"/>
-    </row>
-    <row r="136" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R135" s="7"/>
+      <c r="S135" s="4"/>
+    </row>
+    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A136" s="7"/>
       <c r="B136" s="4"/>
       <c r="C136" s="7"/>
@@ -3806,9 +3979,10 @@
       <c r="O136" s="4"/>
       <c r="P136" s="7"/>
       <c r="Q136" s="7"/>
-      <c r="R136" s="4"/>
-    </row>
-    <row r="137" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R136" s="7"/>
+      <c r="S136" s="4"/>
+    </row>
+    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A137" s="7"/>
       <c r="B137" s="4"/>
       <c r="C137" s="7"/>
@@ -3826,9 +4000,10 @@
       <c r="O137" s="4"/>
       <c r="P137" s="7"/>
       <c r="Q137" s="7"/>
-      <c r="R137" s="4"/>
-    </row>
-    <row r="138" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R137" s="7"/>
+      <c r="S137" s="4"/>
+    </row>
+    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A138" s="7"/>
       <c r="B138" s="4"/>
       <c r="C138" s="7"/>
@@ -3846,9 +4021,10 @@
       <c r="O138" s="4"/>
       <c r="P138" s="7"/>
       <c r="Q138" s="7"/>
-      <c r="R138" s="4"/>
-    </row>
-    <row r="139" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R138" s="7"/>
+      <c r="S138" s="4"/>
+    </row>
+    <row r="139" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A139" s="7"/>
       <c r="B139" s="4"/>
       <c r="C139" s="7"/>
@@ -3866,9 +4042,10 @@
       <c r="O139" s="4"/>
       <c r="P139" s="7"/>
       <c r="Q139" s="7"/>
-      <c r="R139" s="4"/>
-    </row>
-    <row r="140" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R139" s="7"/>
+      <c r="S139" s="4"/>
+    </row>
+    <row r="140" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A140" s="7"/>
       <c r="B140" s="4"/>
       <c r="C140" s="7"/>
@@ -3886,9 +4063,10 @@
       <c r="O140" s="4"/>
       <c r="P140" s="7"/>
       <c r="Q140" s="7"/>
-      <c r="R140" s="4"/>
-    </row>
-    <row r="141" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R140" s="7"/>
+      <c r="S140" s="4"/>
+    </row>
+    <row r="141" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A141" s="7"/>
       <c r="B141" s="4"/>
       <c r="C141" s="7"/>
@@ -3906,9 +4084,10 @@
       <c r="O141" s="4"/>
       <c r="P141" s="7"/>
       <c r="Q141" s="7"/>
-      <c r="R141" s="4"/>
-    </row>
-    <row r="142" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R141" s="7"/>
+      <c r="S141" s="4"/>
+    </row>
+    <row r="142" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A142" s="7"/>
       <c r="B142" s="4"/>
       <c r="C142" s="7"/>
@@ -3926,9 +4105,10 @@
       <c r="O142" s="4"/>
       <c r="P142" s="7"/>
       <c r="Q142" s="7"/>
-      <c r="R142" s="4"/>
-    </row>
-    <row r="143" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R142" s="7"/>
+      <c r="S142" s="4"/>
+    </row>
+    <row r="143" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A143" s="7"/>
       <c r="B143" s="4"/>
       <c r="C143" s="7"/>
@@ -3946,9 +4126,10 @@
       <c r="O143" s="4"/>
       <c r="P143" s="7"/>
       <c r="Q143" s="7"/>
-      <c r="R143" s="4"/>
-    </row>
-    <row r="144" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R143" s="7"/>
+      <c r="S143" s="4"/>
+    </row>
+    <row r="144" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A144" s="7"/>
       <c r="B144" s="4"/>
       <c r="C144" s="7"/>
@@ -3966,9 +4147,10 @@
       <c r="O144" s="4"/>
       <c r="P144" s="7"/>
       <c r="Q144" s="7"/>
-      <c r="R144" s="4"/>
-    </row>
-    <row r="145" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R144" s="7"/>
+      <c r="S144" s="4"/>
+    </row>
+    <row r="145" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A145" s="7"/>
       <c r="B145" s="4"/>
       <c r="C145" s="7"/>
@@ -3986,9 +4168,10 @@
       <c r="O145" s="4"/>
       <c r="P145" s="7"/>
       <c r="Q145" s="7"/>
-      <c r="R145" s="4"/>
-    </row>
-    <row r="146" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R145" s="7"/>
+      <c r="S145" s="4"/>
+    </row>
+    <row r="146" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A146" s="7"/>
       <c r="B146" s="4"/>
       <c r="C146" s="7"/>
@@ -4006,9 +4189,10 @@
       <c r="O146" s="4"/>
       <c r="P146" s="7"/>
       <c r="Q146" s="7"/>
-      <c r="R146" s="4"/>
-    </row>
-    <row r="147" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R146" s="7"/>
+      <c r="S146" s="4"/>
+    </row>
+    <row r="147" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A147" s="7"/>
       <c r="B147" s="4"/>
       <c r="C147" s="7"/>
@@ -4026,9 +4210,10 @@
       <c r="O147" s="4"/>
       <c r="P147" s="7"/>
       <c r="Q147" s="7"/>
-      <c r="R147" s="4"/>
-    </row>
-    <row r="148" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R147" s="7"/>
+      <c r="S147" s="4"/>
+    </row>
+    <row r="148" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A148" s="7"/>
       <c r="B148" s="4"/>
       <c r="C148" s="7"/>
@@ -4046,9 +4231,10 @@
       <c r="O148" s="4"/>
       <c r="P148" s="7"/>
       <c r="Q148" s="7"/>
-      <c r="R148" s="4"/>
-    </row>
-    <row r="149" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R148" s="7"/>
+      <c r="S148" s="4"/>
+    </row>
+    <row r="149" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A149" s="7"/>
       <c r="B149" s="4"/>
       <c r="C149" s="7"/>
@@ -4066,9 +4252,10 @@
       <c r="O149" s="4"/>
       <c r="P149" s="7"/>
       <c r="Q149" s="7"/>
-      <c r="R149" s="4"/>
-    </row>
-    <row r="150" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R149" s="7"/>
+      <c r="S149" s="4"/>
+    </row>
+    <row r="150" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A150" s="7"/>
       <c r="B150" s="4"/>
       <c r="C150" s="7"/>
@@ -4086,9 +4273,10 @@
       <c r="O150" s="4"/>
       <c r="P150" s="7"/>
       <c r="Q150" s="7"/>
-      <c r="R150" s="4"/>
-    </row>
-    <row r="151" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R150" s="7"/>
+      <c r="S150" s="4"/>
+    </row>
+    <row r="151" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A151" s="7"/>
       <c r="B151" s="4"/>
       <c r="C151" s="7"/>
@@ -4106,9 +4294,10 @@
       <c r="O151" s="4"/>
       <c r="P151" s="7"/>
       <c r="Q151" s="7"/>
-      <c r="R151" s="4"/>
-    </row>
-    <row r="152" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R151" s="7"/>
+      <c r="S151" s="4"/>
+    </row>
+    <row r="152" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A152" s="7"/>
       <c r="B152" s="4"/>
       <c r="C152" s="7"/>
@@ -4126,9 +4315,10 @@
       <c r="O152" s="4"/>
       <c r="P152" s="7"/>
       <c r="Q152" s="7"/>
-      <c r="R152" s="4"/>
-    </row>
-    <row r="153" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R152" s="7"/>
+      <c r="S152" s="4"/>
+    </row>
+    <row r="153" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A153" s="7"/>
       <c r="B153" s="4"/>
       <c r="C153" s="7"/>
@@ -4146,9 +4336,10 @@
       <c r="O153" s="4"/>
       <c r="P153" s="7"/>
       <c r="Q153" s="7"/>
-      <c r="R153" s="4"/>
-    </row>
-    <row r="154" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R153" s="7"/>
+      <c r="S153" s="4"/>
+    </row>
+    <row r="154" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A154" s="7"/>
       <c r="B154" s="4"/>
       <c r="C154" s="7"/>
@@ -4166,9 +4357,10 @@
       <c r="O154" s="4"/>
       <c r="P154" s="7"/>
       <c r="Q154" s="7"/>
-      <c r="R154" s="4"/>
-    </row>
-    <row r="155" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R154" s="7"/>
+      <c r="S154" s="4"/>
+    </row>
+    <row r="155" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A155" s="7"/>
       <c r="B155" s="4"/>
       <c r="C155" s="7"/>
@@ -4186,9 +4378,10 @@
       <c r="O155" s="4"/>
       <c r="P155" s="7"/>
       <c r="Q155" s="7"/>
-      <c r="R155" s="4"/>
-    </row>
-    <row r="156" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R155" s="7"/>
+      <c r="S155" s="4"/>
+    </row>
+    <row r="156" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A156" s="7"/>
       <c r="B156" s="4"/>
       <c r="C156" s="7"/>
@@ -4206,9 +4399,10 @@
       <c r="O156" s="4"/>
       <c r="P156" s="7"/>
       <c r="Q156" s="7"/>
-      <c r="R156" s="4"/>
-    </row>
-    <row r="157" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R156" s="7"/>
+      <c r="S156" s="4"/>
+    </row>
+    <row r="157" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A157" s="7"/>
       <c r="B157" s="4"/>
       <c r="C157" s="7"/>
@@ -4226,9 +4420,10 @@
       <c r="O157" s="4"/>
       <c r="P157" s="7"/>
       <c r="Q157" s="7"/>
-      <c r="R157" s="4"/>
-    </row>
-    <row r="158" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R157" s="7"/>
+      <c r="S157" s="4"/>
+    </row>
+    <row r="158" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A158" s="7"/>
       <c r="B158" s="4"/>
       <c r="C158" s="7"/>
@@ -4246,9 +4441,10 @@
       <c r="O158" s="4"/>
       <c r="P158" s="7"/>
       <c r="Q158" s="7"/>
-      <c r="R158" s="4"/>
-    </row>
-    <row r="159" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R158" s="7"/>
+      <c r="S158" s="4"/>
+    </row>
+    <row r="159" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A159" s="7"/>
       <c r="B159" s="4"/>
       <c r="C159" s="7"/>
@@ -4266,9 +4462,10 @@
       <c r="O159" s="4"/>
       <c r="P159" s="7"/>
       <c r="Q159" s="7"/>
-      <c r="R159" s="4"/>
-    </row>
-    <row r="160" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R159" s="7"/>
+      <c r="S159" s="4"/>
+    </row>
+    <row r="160" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A160" s="7"/>
       <c r="B160" s="4"/>
       <c r="C160" s="7"/>
@@ -4286,9 +4483,10 @@
       <c r="O160" s="4"/>
       <c r="P160" s="7"/>
       <c r="Q160" s="7"/>
-      <c r="R160" s="4"/>
-    </row>
-    <row r="161" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R160" s="7"/>
+      <c r="S160" s="4"/>
+    </row>
+    <row r="161" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A161" s="7"/>
       <c r="B161" s="4"/>
       <c r="C161" s="7"/>
@@ -4306,9 +4504,10 @@
       <c r="O161" s="4"/>
       <c r="P161" s="7"/>
       <c r="Q161" s="7"/>
-      <c r="R161" s="4"/>
-    </row>
-    <row r="162" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R161" s="7"/>
+      <c r="S161" s="4"/>
+    </row>
+    <row r="162" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A162" s="7"/>
       <c r="B162" s="4"/>
       <c r="C162" s="7"/>
@@ -4326,9 +4525,10 @@
       <c r="O162" s="4"/>
       <c r="P162" s="7"/>
       <c r="Q162" s="7"/>
-      <c r="R162" s="4"/>
-    </row>
-    <row r="163" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R162" s="7"/>
+      <c r="S162" s="4"/>
+    </row>
+    <row r="163" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A163" s="7"/>
       <c r="B163" s="4"/>
       <c r="C163" s="7"/>
@@ -4346,9 +4546,10 @@
       <c r="O163" s="4"/>
       <c r="P163" s="7"/>
       <c r="Q163" s="7"/>
-      <c r="R163" s="4"/>
-    </row>
-    <row r="164" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R163" s="7"/>
+      <c r="S163" s="4"/>
+    </row>
+    <row r="164" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A164" s="7"/>
       <c r="B164" s="4"/>
       <c r="C164" s="7"/>
@@ -4366,9 +4567,10 @@
       <c r="O164" s="4"/>
       <c r="P164" s="7"/>
       <c r="Q164" s="7"/>
-      <c r="R164" s="4"/>
-    </row>
-    <row r="165" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R164" s="7"/>
+      <c r="S164" s="4"/>
+    </row>
+    <row r="165" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A165" s="7"/>
       <c r="B165" s="4"/>
       <c r="C165" s="7"/>
@@ -4386,9 +4588,10 @@
       <c r="O165" s="4"/>
       <c r="P165" s="7"/>
       <c r="Q165" s="7"/>
-      <c r="R165" s="4"/>
-    </row>
-    <row r="166" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R165" s="7"/>
+      <c r="S165" s="4"/>
+    </row>
+    <row r="166" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A166" s="7"/>
       <c r="B166" s="4"/>
       <c r="C166" s="7"/>
@@ -4406,9 +4609,10 @@
       <c r="O166" s="4"/>
       <c r="P166" s="7"/>
       <c r="Q166" s="7"/>
-      <c r="R166" s="4"/>
-    </row>
-    <row r="167" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R166" s="7"/>
+      <c r="S166" s="4"/>
+    </row>
+    <row r="167" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A167" s="7"/>
       <c r="B167" s="4"/>
       <c r="C167" s="7"/>
@@ -4426,9 +4630,10 @@
       <c r="O167" s="4"/>
       <c r="P167" s="7"/>
       <c r="Q167" s="7"/>
-      <c r="R167" s="4"/>
-    </row>
-    <row r="168" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R167" s="7"/>
+      <c r="S167" s="4"/>
+    </row>
+    <row r="168" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A168" s="7"/>
       <c r="B168" s="4"/>
       <c r="C168" s="7"/>
@@ -4446,9 +4651,10 @@
       <c r="O168" s="4"/>
       <c r="P168" s="7"/>
       <c r="Q168" s="7"/>
-      <c r="R168" s="4"/>
-    </row>
-    <row r="169" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R168" s="7"/>
+      <c r="S168" s="4"/>
+    </row>
+    <row r="169" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A169" s="7"/>
       <c r="B169" s="4"/>
       <c r="C169" s="7"/>
@@ -4466,9 +4672,10 @@
       <c r="O169" s="4"/>
       <c r="P169" s="7"/>
       <c r="Q169" s="7"/>
-      <c r="R169" s="4"/>
-    </row>
-    <row r="170" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R169" s="7"/>
+      <c r="S169" s="4"/>
+    </row>
+    <row r="170" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A170" s="7"/>
       <c r="B170" s="4"/>
       <c r="C170" s="7"/>
@@ -4486,9 +4693,10 @@
       <c r="O170" s="4"/>
       <c r="P170" s="7"/>
       <c r="Q170" s="7"/>
-      <c r="R170" s="4"/>
-    </row>
-    <row r="171" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R170" s="7"/>
+      <c r="S170" s="4"/>
+    </row>
+    <row r="171" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A171" s="7"/>
       <c r="B171" s="4"/>
       <c r="C171" s="7"/>
@@ -4506,9 +4714,10 @@
       <c r="O171" s="4"/>
       <c r="P171" s="7"/>
       <c r="Q171" s="7"/>
-      <c r="R171" s="4"/>
-    </row>
-    <row r="172" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R171" s="7"/>
+      <c r="S171" s="4"/>
+    </row>
+    <row r="172" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A172" s="7"/>
       <c r="B172" s="4"/>
       <c r="C172" s="7"/>
@@ -4526,9 +4735,10 @@
       <c r="O172" s="4"/>
       <c r="P172" s="7"/>
       <c r="Q172" s="7"/>
-      <c r="R172" s="4"/>
-    </row>
-    <row r="173" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R172" s="7"/>
+      <c r="S172" s="4"/>
+    </row>
+    <row r="173" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A173" s="7"/>
       <c r="B173" s="4"/>
       <c r="C173" s="7"/>
@@ -4546,9 +4756,10 @@
       <c r="O173" s="4"/>
       <c r="P173" s="7"/>
       <c r="Q173" s="7"/>
-      <c r="R173" s="4"/>
-    </row>
-    <row r="174" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R173" s="7"/>
+      <c r="S173" s="4"/>
+    </row>
+    <row r="174" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A174" s="7"/>
       <c r="B174" s="4"/>
       <c r="C174" s="7"/>
@@ -4566,9 +4777,10 @@
       <c r="O174" s="4"/>
       <c r="P174" s="7"/>
       <c r="Q174" s="7"/>
-      <c r="R174" s="4"/>
-    </row>
-    <row r="175" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R174" s="7"/>
+      <c r="S174" s="4"/>
+    </row>
+    <row r="175" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A175" s="7"/>
       <c r="B175" s="4"/>
       <c r="C175" s="7"/>
@@ -4586,9 +4798,10 @@
       <c r="O175" s="4"/>
       <c r="P175" s="7"/>
       <c r="Q175" s="7"/>
-      <c r="R175" s="4"/>
-    </row>
-    <row r="176" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R175" s="7"/>
+      <c r="S175" s="4"/>
+    </row>
+    <row r="176" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A176" s="7"/>
       <c r="B176" s="4"/>
       <c r="C176" s="7"/>
@@ -4606,9 +4819,10 @@
       <c r="O176" s="4"/>
       <c r="P176" s="7"/>
       <c r="Q176" s="7"/>
-      <c r="R176" s="4"/>
-    </row>
-    <row r="177" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R176" s="7"/>
+      <c r="S176" s="4"/>
+    </row>
+    <row r="177" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A177" s="7"/>
       <c r="B177" s="4"/>
       <c r="C177" s="7"/>
@@ -4626,9 +4840,10 @@
       <c r="O177" s="4"/>
       <c r="P177" s="7"/>
       <c r="Q177" s="7"/>
-      <c r="R177" s="4"/>
-    </row>
-    <row r="178" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R177" s="7"/>
+      <c r="S177" s="4"/>
+    </row>
+    <row r="178" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A178" s="7"/>
       <c r="B178" s="4"/>
       <c r="C178" s="7"/>
@@ -4646,9 +4861,10 @@
       <c r="O178" s="4"/>
       <c r="P178" s="7"/>
       <c r="Q178" s="7"/>
-      <c r="R178" s="4"/>
-    </row>
-    <row r="179" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R178" s="7"/>
+      <c r="S178" s="4"/>
+    </row>
+    <row r="179" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A179" s="7"/>
       <c r="B179" s="4"/>
       <c r="C179" s="7"/>
@@ -4666,9 +4882,10 @@
       <c r="O179" s="4"/>
       <c r="P179" s="7"/>
       <c r="Q179" s="7"/>
-      <c r="R179" s="4"/>
-    </row>
-    <row r="180" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R179" s="7"/>
+      <c r="S179" s="4"/>
+    </row>
+    <row r="180" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A180" s="7"/>
       <c r="B180" s="4"/>
       <c r="C180" s="7"/>
@@ -4686,9 +4903,10 @@
       <c r="O180" s="4"/>
       <c r="P180" s="7"/>
       <c r="Q180" s="7"/>
-      <c r="R180" s="4"/>
-    </row>
-    <row r="181" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R180" s="7"/>
+      <c r="S180" s="4"/>
+    </row>
+    <row r="181" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A181" s="7"/>
       <c r="B181" s="4"/>
       <c r="C181" s="7"/>
@@ -4706,9 +4924,10 @@
       <c r="O181" s="4"/>
       <c r="P181" s="7"/>
       <c r="Q181" s="7"/>
-      <c r="R181" s="4"/>
-    </row>
-    <row r="182" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R181" s="7"/>
+      <c r="S181" s="4"/>
+    </row>
+    <row r="182" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A182" s="7"/>
       <c r="B182" s="4"/>
       <c r="C182" s="7"/>
@@ -4726,9 +4945,10 @@
       <c r="O182" s="4"/>
       <c r="P182" s="7"/>
       <c r="Q182" s="7"/>
-      <c r="R182" s="4"/>
-    </row>
-    <row r="183" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R182" s="7"/>
+      <c r="S182" s="4"/>
+    </row>
+    <row r="183" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A183" s="7"/>
       <c r="B183" s="4"/>
       <c r="C183" s="7"/>
@@ -4746,9 +4966,10 @@
       <c r="O183" s="4"/>
       <c r="P183" s="7"/>
       <c r="Q183" s="7"/>
-      <c r="R183" s="4"/>
-    </row>
-    <row r="184" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="R183" s="7"/>
+      <c r="S183" s="4"/>
+    </row>
+    <row r="184" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A184" s="7"/>
       <c r="B184" s="4"/>
       <c r="C184" s="7"/>
@@ -4764,9 +4985,9 @@
       <c r="M184" s="7"/>
       <c r="N184" s="5"/>
       <c r="O184" s="4"/>
-      <c r="R184" s="4"/>
-    </row>
-    <row r="185" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S184" s="4"/>
+    </row>
+    <row r="185" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A185" s="7"/>
       <c r="B185" s="4"/>
       <c r="C185" s="7"/>
@@ -4782,9 +5003,9 @@
       <c r="M185" s="7"/>
       <c r="N185" s="5"/>
       <c r="O185" s="4"/>
-      <c r="R185" s="4"/>
-    </row>
-    <row r="186" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S185" s="4"/>
+    </row>
+    <row r="186" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A186" s="7"/>
       <c r="B186" s="4"/>
       <c r="C186" s="7"/>
@@ -4800,9 +5021,9 @@
       <c r="M186" s="7"/>
       <c r="N186" s="5"/>
       <c r="O186" s="4"/>
-      <c r="R186" s="4"/>
-    </row>
-    <row r="187" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S186" s="4"/>
+    </row>
+    <row r="187" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A187" s="7"/>
       <c r="B187" s="4"/>
       <c r="C187" s="7"/>
@@ -4818,9 +5039,9 @@
       <c r="M187" s="7"/>
       <c r="N187" s="5"/>
       <c r="O187" s="4"/>
-      <c r="R187" s="4"/>
-    </row>
-    <row r="188" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S187" s="4"/>
+    </row>
+    <row r="188" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A188" s="7"/>
       <c r="B188" s="4"/>
       <c r="C188" s="7"/>
@@ -4836,9 +5057,9 @@
       <c r="M188" s="7"/>
       <c r="N188" s="5"/>
       <c r="O188" s="4"/>
-      <c r="R188" s="4"/>
-    </row>
-    <row r="189" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S188" s="4"/>
+    </row>
+    <row r="189" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A189" s="7"/>
       <c r="B189" s="4"/>
       <c r="C189" s="7"/>
@@ -4854,9 +5075,9 @@
       <c r="M189" s="7"/>
       <c r="N189" s="5"/>
       <c r="O189" s="4"/>
-      <c r="R189" s="4"/>
-    </row>
-    <row r="190" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S189" s="4"/>
+    </row>
+    <row r="190" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A190" s="7"/>
       <c r="B190" s="4"/>
       <c r="C190" s="7"/>
@@ -4872,9 +5093,9 @@
       <c r="M190" s="7"/>
       <c r="N190" s="5"/>
       <c r="O190" s="4"/>
-      <c r="R190" s="4"/>
-    </row>
-    <row r="191" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S190" s="4"/>
+    </row>
+    <row r="191" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A191" s="7"/>
       <c r="B191" s="4"/>
       <c r="C191" s="7"/>
@@ -4890,9 +5111,9 @@
       <c r="M191" s="7"/>
       <c r="N191" s="5"/>
       <c r="O191" s="4"/>
-      <c r="R191" s="4"/>
-    </row>
-    <row r="192" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S191" s="4"/>
+    </row>
+    <row r="192" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A192" s="7"/>
       <c r="B192" s="4"/>
       <c r="C192" s="7"/>
@@ -4908,9 +5129,9 @@
       <c r="M192" s="7"/>
       <c r="N192" s="5"/>
       <c r="O192" s="4"/>
-      <c r="R192" s="4"/>
-    </row>
-    <row r="193" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S192" s="4"/>
+    </row>
+    <row r="193" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A193" s="7"/>
       <c r="B193" s="4"/>
       <c r="C193" s="7"/>
@@ -4926,9 +5147,9 @@
       <c r="M193" s="7"/>
       <c r="N193" s="5"/>
       <c r="O193" s="4"/>
-      <c r="R193" s="4"/>
-    </row>
-    <row r="194" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S193" s="4"/>
+    </row>
+    <row r="194" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A194" s="7"/>
       <c r="B194" s="4"/>
       <c r="C194" s="7"/>
@@ -4944,9 +5165,9 @@
       <c r="M194" s="7"/>
       <c r="N194" s="5"/>
       <c r="O194" s="4"/>
-      <c r="R194" s="4"/>
-    </row>
-    <row r="195" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S194" s="4"/>
+    </row>
+    <row r="195" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A195" s="7"/>
       <c r="B195" s="4"/>
       <c r="C195" s="7"/>
@@ -4962,9 +5183,9 @@
       <c r="M195" s="7"/>
       <c r="N195" s="5"/>
       <c r="O195" s="4"/>
-      <c r="R195" s="4"/>
-    </row>
-    <row r="196" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S195" s="4"/>
+    </row>
+    <row r="196" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A196" s="7"/>
       <c r="B196" s="4"/>
       <c r="C196" s="7"/>
@@ -4980,9 +5201,9 @@
       <c r="M196" s="7"/>
       <c r="N196" s="5"/>
       <c r="O196" s="4"/>
-      <c r="R196" s="4"/>
-    </row>
-    <row r="197" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S196" s="4"/>
+    </row>
+    <row r="197" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A197" s="7"/>
       <c r="B197" s="4"/>
       <c r="C197" s="7"/>
@@ -4998,9 +5219,9 @@
       <c r="M197" s="7"/>
       <c r="N197" s="5"/>
       <c r="O197" s="4"/>
-      <c r="R197" s="4"/>
-    </row>
-    <row r="198" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S197" s="4"/>
+    </row>
+    <row r="198" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A198" s="7"/>
       <c r="B198" s="4"/>
       <c r="C198" s="7"/>
@@ -5016,9 +5237,9 @@
       <c r="M198" s="7"/>
       <c r="N198" s="5"/>
       <c r="O198" s="4"/>
-      <c r="R198" s="4"/>
-    </row>
-    <row r="199" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S198" s="4"/>
+    </row>
+    <row r="199" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A199" s="7"/>
       <c r="B199" s="4"/>
       <c r="C199" s="7"/>
@@ -5034,9 +5255,9 @@
       <c r="M199" s="7"/>
       <c r="N199" s="5"/>
       <c r="O199" s="4"/>
-      <c r="R199" s="4"/>
-    </row>
-    <row r="200" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S199" s="4"/>
+    </row>
+    <row r="200" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A200" s="7"/>
       <c r="B200" s="4"/>
       <c r="C200" s="7"/>
@@ -5052,9 +5273,9 @@
       <c r="M200" s="7"/>
       <c r="N200" s="5"/>
       <c r="O200" s="4"/>
-      <c r="R200" s="4"/>
-    </row>
-    <row r="201" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S200" s="4"/>
+    </row>
+    <row r="201" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A201" s="7"/>
       <c r="B201" s="4"/>
       <c r="C201" s="7"/>
@@ -5070,9 +5291,9 @@
       <c r="M201" s="7"/>
       <c r="N201" s="5"/>
       <c r="O201" s="4"/>
-      <c r="R201" s="4"/>
-    </row>
-    <row r="202" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S201" s="4"/>
+    </row>
+    <row r="202" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A202" s="7"/>
       <c r="B202" s="4"/>
       <c r="C202" s="7"/>
@@ -5088,9 +5309,9 @@
       <c r="M202" s="7"/>
       <c r="N202" s="5"/>
       <c r="O202" s="4"/>
-      <c r="R202" s="4"/>
-    </row>
-    <row r="203" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S202" s="4"/>
+    </row>
+    <row r="203" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A203" s="7"/>
       <c r="B203" s="4"/>
       <c r="C203" s="7"/>
@@ -5106,9 +5327,9 @@
       <c r="M203" s="7"/>
       <c r="N203" s="5"/>
       <c r="O203" s="4"/>
-      <c r="R203" s="4"/>
-    </row>
-    <row r="204" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S203" s="4"/>
+    </row>
+    <row r="204" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A204" s="7"/>
       <c r="B204" s="4"/>
       <c r="C204" s="7"/>
@@ -5124,9 +5345,9 @@
       <c r="M204" s="7"/>
       <c r="N204" s="5"/>
       <c r="O204" s="4"/>
-      <c r="R204" s="4"/>
-    </row>
-    <row r="205" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S204" s="4"/>
+    </row>
+    <row r="205" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A205" s="7"/>
       <c r="B205" s="4"/>
       <c r="C205" s="7"/>
@@ -5142,9 +5363,9 @@
       <c r="M205" s="7"/>
       <c r="N205" s="5"/>
       <c r="O205" s="4"/>
-      <c r="R205" s="4"/>
-    </row>
-    <row r="206" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S205" s="4"/>
+    </row>
+    <row r="206" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A206" s="7"/>
       <c r="B206" s="4"/>
       <c r="C206" s="7"/>
@@ -5160,9 +5381,9 @@
       <c r="M206" s="7"/>
       <c r="N206" s="5"/>
       <c r="O206" s="4"/>
-      <c r="R206" s="4"/>
-    </row>
-    <row r="207" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S206" s="4"/>
+    </row>
+    <row r="207" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A207" s="7"/>
       <c r="B207" s="4"/>
       <c r="C207" s="7"/>
@@ -5178,9 +5399,9 @@
       <c r="M207" s="7"/>
       <c r="N207" s="5"/>
       <c r="O207" s="4"/>
-      <c r="R207" s="4"/>
-    </row>
-    <row r="208" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S207" s="4"/>
+    </row>
+    <row r="208" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A208" s="7"/>
       <c r="B208" s="4"/>
       <c r="C208" s="7"/>
@@ -5196,9 +5417,9 @@
       <c r="M208" s="7"/>
       <c r="N208" s="5"/>
       <c r="O208" s="4"/>
-      <c r="R208" s="4"/>
-    </row>
-    <row r="209" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S208" s="4"/>
+    </row>
+    <row r="209" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A209" s="7"/>
       <c r="B209" s="4"/>
       <c r="C209" s="7"/>
@@ -5214,9 +5435,9 @@
       <c r="M209" s="7"/>
       <c r="N209" s="5"/>
       <c r="O209" s="4"/>
-      <c r="R209" s="4"/>
-    </row>
-    <row r="210" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S209" s="4"/>
+    </row>
+    <row r="210" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A210" s="7"/>
       <c r="B210" s="4"/>
       <c r="C210" s="7"/>
@@ -5232,9 +5453,9 @@
       <c r="M210" s="7"/>
       <c r="N210" s="5"/>
       <c r="O210" s="4"/>
-      <c r="R210" s="4"/>
-    </row>
-    <row r="211" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S210" s="4"/>
+    </row>
+    <row r="211" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A211" s="7"/>
       <c r="B211" s="4"/>
       <c r="C211" s="7"/>
@@ -5250,9 +5471,9 @@
       <c r="M211" s="7"/>
       <c r="N211" s="5"/>
       <c r="O211" s="4"/>
-      <c r="R211" s="4"/>
-    </row>
-    <row r="212" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S211" s="4"/>
+    </row>
+    <row r="212" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A212" s="7"/>
       <c r="B212" s="4"/>
       <c r="C212" s="7"/>
@@ -5268,9 +5489,9 @@
       <c r="M212" s="7"/>
       <c r="N212" s="5"/>
       <c r="O212" s="4"/>
-      <c r="R212" s="4"/>
-    </row>
-    <row r="213" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S212" s="4"/>
+    </row>
+    <row r="213" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A213" s="7"/>
       <c r="B213" s="4"/>
       <c r="C213" s="7"/>
@@ -5286,9 +5507,9 @@
       <c r="M213" s="7"/>
       <c r="N213" s="5"/>
       <c r="O213" s="4"/>
-      <c r="R213" s="4"/>
-    </row>
-    <row r="214" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S213" s="4"/>
+    </row>
+    <row r="214" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A214" s="7"/>
       <c r="B214" s="4"/>
       <c r="C214" s="7"/>
@@ -5304,9 +5525,9 @@
       <c r="M214" s="7"/>
       <c r="N214" s="5"/>
       <c r="O214" s="4"/>
-      <c r="R214" s="4"/>
-    </row>
-    <row r="215" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S214" s="4"/>
+    </row>
+    <row r="215" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A215" s="7"/>
       <c r="B215" s="4"/>
       <c r="C215" s="7"/>
@@ -5322,9 +5543,9 @@
       <c r="M215" s="7"/>
       <c r="N215" s="5"/>
       <c r="O215" s="4"/>
-      <c r="R215" s="4"/>
-    </row>
-    <row r="216" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S215" s="4"/>
+    </row>
+    <row r="216" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A216" s="7"/>
       <c r="B216" s="4"/>
       <c r="C216" s="7"/>
@@ -5340,9 +5561,9 @@
       <c r="M216" s="7"/>
       <c r="N216" s="5"/>
       <c r="O216" s="4"/>
-      <c r="R216" s="4"/>
-    </row>
-    <row r="217" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S216" s="4"/>
+    </row>
+    <row r="217" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A217" s="7"/>
       <c r="B217" s="4"/>
       <c r="C217" s="7"/>
@@ -5358,9 +5579,9 @@
       <c r="M217" s="7"/>
       <c r="N217" s="5"/>
       <c r="O217" s="4"/>
-      <c r="R217" s="4"/>
-    </row>
-    <row r="218" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S217" s="4"/>
+    </row>
+    <row r="218" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A218" s="7"/>
       <c r="B218" s="4"/>
       <c r="C218" s="7"/>
@@ -5376,7 +5597,7 @@
       <c r="M218" s="7"/>
       <c r="N218" s="5"/>
       <c r="O218" s="4"/>
-      <c r="R218" s="4"/>
+      <c r="S218" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -5393,18 +5614,18 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="43.25" customWidth="1"/>
+    <col min="2" max="2" width="43.21875" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="20.625" customWidth="1"/>
-    <col min="7" max="7" width="42.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.25" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" customWidth="1"/>
+    <col min="7" max="7" width="42.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>19</v>
       </c>
@@ -5430,7 +5651,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
@@ -5440,7 +5661,7 @@
       <c r="G2" s="26"/>
       <c r="H2" s="26"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="25"/>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
@@ -5450,7 +5671,7 @@
       <c r="G3" s="25"/>
       <c r="H3" s="25"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="25"/>
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
@@ -5460,7 +5681,7 @@
       <c r="G4" s="25"/>
       <c r="H4" s="25"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="25"/>
       <c r="B5" s="25"/>
       <c r="C5" s="25"/>
@@ -5470,7 +5691,7 @@
       <c r="G5" s="25"/>
       <c r="H5" s="25"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="25"/>
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
@@ -5480,7 +5701,7 @@
       <c r="G6" s="25"/>
       <c r="H6" s="25"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="25"/>
       <c r="B7" s="25"/>
       <c r="C7" s="25"/>
@@ -5490,7 +5711,7 @@
       <c r="G7" s="25"/>
       <c r="H7" s="25"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="25"/>
       <c r="B8" s="25"/>
       <c r="C8" s="25"/>
@@ -5500,7 +5721,7 @@
       <c r="G8" s="25"/>
       <c r="H8" s="25"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="25"/>
       <c r="B9" s="25"/>
       <c r="C9" s="25"/>
@@ -5510,7 +5731,7 @@
       <c r="G9" s="25"/>
       <c r="H9" s="25"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="25"/>
       <c r="B10" s="25"/>
       <c r="C10" s="25"/>
@@ -5520,7 +5741,7 @@
       <c r="G10" s="25"/>
       <c r="H10" s="25"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="25"/>
       <c r="B11" s="25"/>
       <c r="C11" s="25"/>
@@ -5530,7 +5751,7 @@
       <c r="G11" s="25"/>
       <c r="H11" s="25"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="25"/>
       <c r="B12" s="25"/>
       <c r="C12" s="25"/>
@@ -5540,7 +5761,7 @@
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="25"/>
       <c r="B13" s="25"/>
       <c r="C13" s="25"/>
@@ -5550,7 +5771,7 @@
       <c r="G13" s="25"/>
       <c r="H13" s="25"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="25"/>
       <c r="B14" s="25"/>
       <c r="C14" s="25"/>
@@ -5560,7 +5781,7 @@
       <c r="G14" s="25"/>
       <c r="H14" s="25"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="25"/>
       <c r="B15" s="25"/>
       <c r="C15" s="25"/>
@@ -5570,7 +5791,7 @@
       <c r="G15" s="25"/>
       <c r="H15" s="25"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="25"/>
       <c r="B16" s="25"/>
       <c r="C16" s="25"/>
@@ -5580,7 +5801,7 @@
       <c r="G16" s="25"/>
       <c r="H16" s="25"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="25"/>
       <c r="B17" s="25"/>
       <c r="C17" s="25"/>
@@ -5590,7 +5811,7 @@
       <c r="G17" s="25"/>
       <c r="H17" s="25"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="25"/>
       <c r="B18" s="25"/>
       <c r="C18" s="25"/>
@@ -5600,7 +5821,7 @@
       <c r="G18" s="25"/>
       <c r="H18" s="25"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="25"/>
       <c r="B19" s="25"/>
       <c r="C19" s="25"/>

</xml_diff>